<commit_message>
add pso whit 2 varable
</commit_message>
<xml_diff>
--- a/Resultados/resultados PSO simple 12_06_23.xlsx
+++ b/Resultados/resultados PSO simple 12_06_23.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Universidad\Proyecto titulo1\PSO\Resultados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3797E454-906D-4E74-8A4D-23694F9CCBDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50C6CAFF-5BB5-4BF4-B496-AA09C750B79D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="#,##0.000"/>
+    <numFmt numFmtId="164" formatCode="#,##0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -80,7 +80,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -113,6 +113,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-CL"/>
+              <a:t>Función</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-CL" baseline="0"/>
+              <a:t> 2</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-CL"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -654,7 +684,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="es-CL"/>
-                  <a:t>Valor particula</a:t>
+                  <a:t>Valor partícula</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1631,7 +1661,7 @@
   <dimension ref="A1:C52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>